<commit_message>
Added metadata on soil samples texture group and individual measurements in last samples
</commit_message>
<xml_diff>
--- a/experiment_metadata.xlsx
+++ b/experiment_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcajasmunoz/Library/CloudStorage/GoogleDrive-dadavid.cajas@gmail.com/Mi unidad/Academia/Postgrado/UvA/Results and experiments track/Experiment 1 - Inoculants and amendments on crops and grasses/9-Analysis/Microresp/Samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcajasmunoz/Library/CloudStorage/GoogleDrive-dadavid.cajas@gmail.com/Mi unidad/Academia/Postgrado/UvA/Results and experiments track/Experiment 1 - Inoculants and amendments on crops and grasses/9-Analysis/3-Pathogen growth inhibition/R/Pathogen_inhibition_pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377E7D44-69F6-9D4F-97C6-939A260EB8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B20D23A-ADDD-9F41-87FE-A8CABFFA82FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14700" yWindow="740" windowWidth="19860" windowHeight="21600" xr2:uid="{A6F77838-32D7-9847-A48C-CD707F284975}"/>
+    <workbookView xWindow="14700" yWindow="760" windowWidth="19860" windowHeight="21580" xr2:uid="{A6F77838-32D7-9847-A48C-CD707F284975}"/>
   </bookViews>
   <sheets>
     <sheet name="soil_data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="149">
   <si>
     <t>Hoge eng</t>
   </si>
@@ -472,9 +472,6 @@
     <t>origin_location</t>
   </si>
   <si>
-    <t>soil_texture</t>
-  </si>
-  <si>
     <t>applied_product</t>
   </si>
   <si>
@@ -482,6 +479,12 @@
   </si>
   <si>
     <t>treatment_provider</t>
+  </si>
+  <si>
+    <t>soil_texture_main</t>
+  </si>
+  <si>
+    <t>soil_texture_sub</t>
   </si>
 </sst>
 </file>
@@ -883,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3CA777-69F1-8E4A-8F38-08C59349FDCA}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,19 +899,19 @@
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -925,37 +928,40 @@
         <v>122</v>
       </c>
       <c r="F1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -972,37 +978,40 @@
         <v>5.5767829999999998</v>
       </c>
       <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
         <v>39</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>40</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>33</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>18</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>231</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1021,35 +1030,38 @@
       <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3">
         <v>92</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>14</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>402</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1066,37 +1078,40 @@
         <v>6.2304690000000003</v>
       </c>
       <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
         <v>41</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>63</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>17</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>14</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>17</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>19</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1113,33 +1128,36 @@
         <v>5.6700749999999998</v>
       </c>
       <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>78</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>14</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>4</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>8</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>12</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>16</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>100</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1180,10 +1198,10 @@
         <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E1" t="s">
         <v>98</v>
@@ -1542,7 +1560,7 @@
         <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
         <v>82</v>

</xml_diff>